<commit_message>
finally placed all the daeths
</commit_message>
<xml_diff>
--- a/src/syria_under_reporting/death_sheet.xlsx
+++ b/src/syria_under_reporting/death_sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Dam</t>
   </si>
   <si>
+    <t xml:space="preserve">Rif</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sweida</t>
   </si>
   <si>
@@ -62,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://sana.sy/en/?p=195773</t>
   </si>
   <si>
     <r>
@@ -227,7 +233,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -270,6 +276,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -349,12 +359,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -380,7 +390,7 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
@@ -389,13 +399,13 @@
       <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="6" t="s">
@@ -404,216 +414,243 @@
       <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
-        <v>44060</v>
+        <v>44061</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" s="6"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5"/>
       <c r="L2" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="M2" s="5" t="n">
-        <f aca="false">IF(SUM(D2:L2)=C2,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="N2" s="5"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="5" t="n">
+        <f aca="false">IF(SUM(D2:M2)=C2,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="n">
-        <v>44059</v>
-      </c>
-      <c r="B3" s="8" t="n">
-        <v>64</v>
-      </c>
-      <c r="C3" s="9" t="n">
-        <f aca="false">B3-B4</f>
+        <v>44060</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="C3" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D3" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="5"/>
+      <c r="D3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="6"/>
       <c r="K3" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5" t="n">
-        <f aca="false">IF(SUM(D3:L3)=C3,1,0)</f>
-        <v>1</v>
-      </c>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="5" t="n">
+        <f aca="false">IF(SUM(D3:M3)=C3,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
-        <v>44058</v>
+        <v>44059</v>
       </c>
       <c r="B4" s="8" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C4" s="9" t="n">
         <f aca="false">B4-B5</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="5"/>
+      <c r="H4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6"/>
       <c r="J4" s="5" t="n">
         <v>1</v>
       </c>
       <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5" t="n">
-        <f aca="false">IF(SUM(D4:L4)=C4,1,0)</f>
+      <c r="L4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5" t="n">
+        <f aca="false">IF(SUM(D4:M4)=C4,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="n">
-        <v>44057</v>
+        <v>44058</v>
       </c>
       <c r="B5" s="8" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C5" s="9" t="n">
         <f aca="false">B5-B6</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>1</v>
-      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="I5" s="6"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
+      <c r="K5" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="L5" s="5"/>
-      <c r="M5" s="5" t="n">
-        <f aca="false">IF(SUM(D5:L5)=C5,1,0)</f>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5" t="n">
+        <f aca="false">IF(SUM(D5:M5)=C5,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="n">
-        <v>44056</v>
+        <v>44057</v>
       </c>
       <c r="B6" s="8" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C6" s="9" t="n">
         <f aca="false">B6-B7</f>
-        <v>2</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="D6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="5" t="n">
-        <f aca="false">IF(SUM(D6:L6)=C6,1,0)</f>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5" t="n">
+        <f aca="false">IF(SUM(D6:M6)=C6,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="B7" s="8" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C7" s="9" t="n">
         <f aca="false">B7-B8</f>
-        <v>1</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="D7" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="5" t="n">
+        <v>2</v>
+      </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="5" t="n">
-        <f aca="false">IF(SUM(D7:L7)=C7,1,0)</f>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5" t="n">
+        <f aca="false">IF(SUM(D7:M7)=C7,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="B8" s="8" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" s="9" t="n">
         <f aca="false">B8-B9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="M8" s="5" t="n">
-        <f aca="false">IF(SUM(D8:L8)=C8,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5" t="n">
+        <f aca="false">IF(SUM(D8:M8)=C8,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="n">
-        <v>44051</v>
+        <v>44052</v>
       </c>
       <c r="B9" s="8" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C9" s="9" t="n">
         <f aca="false">B9-B10</f>
@@ -622,180 +659,198 @@
       <c r="D9" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="M9" s="5" t="n">
-        <f aca="false">IF(SUM(D9:L9)=C9,1,0)</f>
+      <c r="E9" s="10"/>
+      <c r="F9" s="5"/>
+      <c r="N9" s="5" t="n">
+        <f aca="false">IF(SUM(D9:M9)=C9,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="n">
-        <v>44048</v>
+        <v>44051</v>
       </c>
       <c r="B10" s="8" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C10" s="9" t="n">
         <f aca="false">B10-B11</f>
         <v>2</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="F10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M10" s="5" t="n">
-        <f aca="false">IF(SUM(D10:L10)=C10,1,0)</f>
+      <c r="D10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="H10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N10" s="5" t="n">
+        <f aca="false">IF(SUM(D10:M10)=C10,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="n">
-        <v>44046</v>
+        <v>44048</v>
       </c>
       <c r="B11" s="8" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C11" s="9" t="n">
         <f aca="false">B11-B12</f>
         <v>2</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="D11" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="10"/>
       <c r="G11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="M11" s="5" t="n">
-        <f aca="false">IF(SUM(D11:L11)=C11,1,0)</f>
+      <c r="H11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" s="5" t="n">
+        <f aca="false">IF(SUM(D11:M11)=C11,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="B12" s="8" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C12" s="9" t="n">
         <f aca="false">B12-B13</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="M12" s="5" t="n">
-        <f aca="false">IF(SUM(D12:L12)=C12,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" s="5" t="n">
+        <f aca="false">IF(SUM(D12:M12)=C12,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="B13" s="8" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C13" s="9" t="n">
-        <f aca="false">B13-B14</f>
         <v>1</v>
       </c>
       <c r="D13" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="M13" s="5" t="n">
-        <f aca="false">IF(SUM(D13:L13)=C13,1,0)</f>
+      <c r="E13" s="10"/>
+      <c r="N13" s="5" t="n">
+        <f aca="false">IF(SUM(D13:M13)=C13,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="n">
-        <v>44039</v>
+        <v>44043</v>
       </c>
       <c r="B14" s="8" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C14" s="9" t="n">
-        <f aca="false">B14-B15</f>
         <v>2</v>
       </c>
       <c r="D14" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="M14" s="5" t="n">
-        <f aca="false">IF(SUM(D14:L14)=C14,1,0)</f>
-        <v>1</v>
-      </c>
+      <c r="E14" s="10"/>
+      <c r="N14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="n">
-        <v>44038</v>
+        <v>44042</v>
       </c>
       <c r="B15" s="8" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C15" s="9" t="n">
         <f aca="false">B15-B16</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M15" s="5" t="n">
-        <f aca="false">IF(SUM(D15:L15)=C15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="10"/>
+      <c r="N15" s="5" t="n">
+        <f aca="false">IF(SUM(D15:M15)=C15,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="n">
-        <v>44037</v>
+        <v>44039</v>
       </c>
       <c r="B16" s="8" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C16" s="9" t="n">
         <f aca="false">B16-B17</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="M16" s="5" t="n">
-        <f aca="false">IF(SUM(D16:L16)=C16,1,0)</f>
-        <v>1</v>
+      <c r="E16" s="10"/>
+      <c r="K16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" s="5" t="n">
+        <f aca="false">IF(SUM(D16:M16)=C16,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O16" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="n">
-        <v>44035</v>
+        <v>44038</v>
       </c>
       <c r="B17" s="8" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C17" s="9" t="n">
         <f aca="false">B17-B18</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="M17" s="5" t="n">
-        <f aca="false">IF(SUM(D17:L17)=C17,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" s="5" t="n">
+        <f aca="false">IF(SUM(D17:M17)=C17,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="n">
-        <v>44034</v>
+        <v>44037</v>
       </c>
       <c r="B18" s="8" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C18" s="9" t="n">
         <f aca="false">B18-B19</f>
@@ -804,134 +859,140 @@
       <c r="D18" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="M18" s="5" t="n">
-        <f aca="false">IF(SUM(D18:L18)=C18,1,0)</f>
+      <c r="E18" s="10"/>
+      <c r="N18" s="5" t="n">
+        <f aca="false">IF(SUM(D18:M18)=C18,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="n">
-        <v>44033</v>
+        <v>44035</v>
       </c>
       <c r="B19" s="8" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C19" s="9" t="n">
         <f aca="false">B19-B20</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="M19" s="5" t="n">
-        <f aca="false">IF(SUM(D19:L19)=C19,1,0)</f>
+        <v>3</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="N19" s="5" t="n">
+        <f aca="false">IF(SUM(D19:M19)=C19,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="B20" s="8" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C20" s="9" t="n">
         <f aca="false">B20-B21</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D20" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="M20" s="5" t="n">
-        <f aca="false">IF(SUM(D20:L20)=C20,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="N20" s="5" t="n">
+        <f aca="false">IF(SUM(D20:M20)=C20,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="n">
-        <v>44029</v>
+        <v>44033</v>
       </c>
       <c r="B21" s="8" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C21" s="9" t="n">
         <f aca="false">B21-B22</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="H21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M21" s="5" t="n">
-        <f aca="false">IF(SUM(D21:L21)=C21,1,0)</f>
+      <c r="E21" s="10"/>
+      <c r="N21" s="5" t="n">
+        <f aca="false">IF(SUM(D21:M21)=C21,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="n">
-        <v>44027</v>
+        <v>44032</v>
       </c>
       <c r="B22" s="8" t="n">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C22" s="9" t="n">
         <f aca="false">B22-B23</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D22" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M22" s="5" t="n">
-        <f aca="false">IF(SUM(D22:L22)=C22,1,0)</f>
+        <v>4</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="N22" s="5" t="n">
+        <f aca="false">IF(SUM(D22:M22)=C22,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="n">
-        <v>44026</v>
+        <v>44029</v>
       </c>
       <c r="B23" s="8" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C23" s="9" t="n">
         <f aca="false">B23-B24</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D23" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="M23" s="5" t="n">
-        <f aca="false">IF(SUM(D23:L23)=C23,1,0)</f>
+        <v>3</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="N23" s="5" t="n">
+        <f aca="false">IF(SUM(D23:M23)=C23,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="n">
-        <v>44025</v>
+        <v>44027</v>
       </c>
       <c r="B24" s="8" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C24" s="9" t="n">
         <f aca="false">B24-B25</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D24" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="M24" s="5" t="n">
-        <f aca="false">IF(SUM(D24:L24)=C24,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="N24" s="5" t="n">
+        <f aca="false">IF(SUM(D24:M24)=C24,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="n">
-        <v>44022</v>
+        <v>44026</v>
       </c>
       <c r="B25" s="8" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C25" s="9" t="n">
         <f aca="false">B25-B26</f>
@@ -940,55 +1001,58 @@
       <c r="D25" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="M25" s="5" t="n">
-        <f aca="false">IF(SUM(D25:L25)=C25,1,0)</f>
+      <c r="E25" s="10"/>
+      <c r="N25" s="5" t="n">
+        <f aca="false">IF(SUM(D25:M25)=C25,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="n">
-        <v>44018</v>
+        <v>44025</v>
       </c>
       <c r="B26" s="8" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C26" s="9" t="n">
         <f aca="false">B26-B27</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D26" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M26" s="5" t="n">
-        <f aca="false">IF(SUM(D26:L26)=C26,1,0)</f>
+        <v>3</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="N26" s="5" t="n">
+        <f aca="false">IF(SUM(D26:M26)=C26,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="n">
-        <v>44017</v>
+        <v>44022</v>
       </c>
       <c r="B27" s="8" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C27" s="9" t="n">
         <f aca="false">B27-B28</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="M27" s="5" t="n">
-        <f aca="false">IF(SUM(D27:L27)=C27,1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="N27" s="5" t="n">
+        <f aca="false">IF(SUM(D27:M27)=C27,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="n">
-        <v>44015</v>
+        <v>44018</v>
       </c>
       <c r="B28" s="8" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C28" s="9" t="n">
         <f aca="false">B28-B29</f>
@@ -997,40 +1061,40 @@
       <c r="D28" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="M28" s="5" t="n">
-        <f aca="false">IF(SUM(D28:L28)=C28,1,0)</f>
+      <c r="E28" s="10"/>
+      <c r="N28" s="5" t="n">
+        <f aca="false">IF(SUM(D28:M28)=C28,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="n">
-        <v>44009</v>
+        <v>44017</v>
       </c>
       <c r="B29" s="8" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C29" s="9" t="n">
         <f aca="false">B29-B30</f>
-        <v>1</v>
-      </c>
-      <c r="D29" s="10"/>
-      <c r="J29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M29" s="5" t="n">
-        <f aca="false">IF(SUM(D29:L29)=C29,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="N29" s="10" t="s">
-        <v>14</v>
+        <v>3</v>
+      </c>
+      <c r="D29" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="N29" s="5" t="n">
+        <f aca="false">IF(SUM(D29:M29)=C29,1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="n">
-        <v>44008</v>
+        <v>44015</v>
       </c>
       <c r="B30" s="8" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C30" s="9" t="n">
         <f aca="false">B30-B31</f>
@@ -1039,36 +1103,44 @@
       <c r="D30" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="M30" s="5" t="n">
-        <f aca="false">IF(SUM(D30:L30)=C30,1,0)</f>
+      <c r="E30" s="10"/>
+      <c r="N30" s="5" t="n">
+        <f aca="false">IF(SUM(D30:M30)=C30,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="n">
-        <v>43989</v>
+        <v>44009</v>
       </c>
       <c r="B31" s="8" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C31" s="9" t="n">
         <f aca="false">B31-B32</f>
         <v>1</v>
       </c>
       <c r="D31" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M31" s="5" t="n">
-        <f aca="false">IF(SUM(D31:L31)=C31,1,0)</f>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="K31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N31" s="5" t="n">
+        <f aca="false">IF(SUM(D31:M31)=C31,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O31" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="n">
-        <v>43984</v>
+        <v>44008</v>
       </c>
       <c r="B32" s="8" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C32" s="9" t="n">
         <f aca="false">B32-B33</f>
@@ -1077,36 +1149,41 @@
       <c r="D32" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="M32" s="5" t="n">
-        <f aca="false">IF(SUM(D32:L32)=C32,1,0)</f>
+      <c r="E32" s="10"/>
+      <c r="N32" s="5" t="n">
+        <f aca="false">IF(SUM(D32:M32)=C32,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="n">
-        <v>43982</v>
+        <v>43999</v>
       </c>
       <c r="B33" s="8" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C33" s="9" t="n">
         <f aca="false">B33-B34</f>
         <v>1</v>
       </c>
       <c r="D33" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M33" s="5" t="n">
-        <f aca="false">IF(SUM(D33:L33)=C33,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="I33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N33" s="5" t="n">
+        <f aca="false">IF(SUM(D33:M33)=C33,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="n">
-        <v>43973</v>
+        <v>43984</v>
       </c>
       <c r="B34" s="8" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C34" s="9" t="n">
         <f aca="false">B34-B35</f>
@@ -1115,45 +1192,158 @@
       <c r="D34" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="M34" s="5" t="n">
-        <f aca="false">IF(SUM(D34:L34)=C34,1,0)</f>
+      <c r="E34" s="10"/>
+      <c r="N34" s="5" t="n">
+        <f aca="false">IF(SUM(D34:M34)=C34,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="n">
-        <v>43940</v>
+        <v>43982</v>
       </c>
       <c r="B35" s="8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C35" s="9" t="n">
+        <f aca="false">B35-B36</f>
         <v>1</v>
       </c>
       <c r="D35" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="M35" s="5" t="n">
-        <f aca="false">IF(SUM(D35:L35)=C35,1,0)</f>
+      <c r="E35" s="10"/>
+      <c r="N35" s="5" t="n">
+        <f aca="false">IF(SUM(D35:M35)=C35,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="n">
-        <v>43928</v>
+        <v>43973</v>
       </c>
       <c r="B36" s="8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C36" s="9" t="n">
-        <v>2</v>
+        <f aca="false">B36-B37</f>
+        <v>1</v>
       </c>
       <c r="D36" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="M36" s="5" t="n">
-        <f aca="false">IF(SUM(D36:L36)=C36,1,0)</f>
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="N36" s="5" t="n">
+        <f aca="false">IF(SUM(D36:M36)=C36,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7" t="n">
+        <v>43940</v>
+      </c>
+      <c r="B37" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C37" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="N37" s="5" t="n">
+        <f aca="false">IF(SUM(D37:M37)=C37,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7" t="n">
+        <v>43920</v>
+      </c>
+      <c r="B38" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C38" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="N38" s="5" t="n">
+        <f aca="false">IF(SUM(D38:M38)=C38,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7" t="n">
+        <v>43919</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N39" s="5" t="n">
+        <f aca="false">IF(SUM(D39:M39)=C39,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="1" t="n">
+        <f aca="false">SUM(C3:C39)</f>
+        <v>68</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <f aca="false">SUM(D3:D39)</f>
+        <v>44</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <f aca="false">SUM(E3:E39)</f>
+        <v>3</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <f aca="false">SUM(F3:F39)</f>
+        <v>6</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <f aca="false">SUM(G3:G39)</f>
+        <v>2</v>
+      </c>
+      <c r="H40" s="1" t="n">
+        <f aca="false">SUM(H3:H39)</f>
+        <v>5</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <f aca="false">SUM(I3:I39)</f>
+        <v>1</v>
+      </c>
+      <c r="J40" s="1" t="n">
+        <f aca="false">SUM(J3:J39)</f>
+        <v>1</v>
+      </c>
+      <c r="K40" s="1" t="n">
+        <f aca="false">SUM(K3:K39)</f>
+        <v>4</v>
+      </c>
+      <c r="L40" s="1" t="n">
+        <f aca="false">SUM(L3:L39)</f>
+        <v>1</v>
+      </c>
+      <c r="M40" s="1" t="n">
+        <f aca="false">SUM(M3:M39)</f>
+        <v>1</v>
+      </c>
+      <c r="N40" s="0" t="n">
+        <f aca="false">SUM(D40:M40)</f>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
syria update data and initts for late start
</commit_message>
<xml_diff>
--- a/src/syria_under_reporting/death_sheet.xlsx
+++ b/src/syria_under_reporting/death_sheet.xlsx
@@ -78,7 +78,7 @@
         <sz val="12"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="128"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1 Aleppo *1</t>
     </r>
@@ -88,7 +88,7 @@
         <sz val="12"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="128"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">st</t>
     </r>
@@ -97,7 +97,7 @@
         <sz val="12"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="128"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> recorded Aleppo case</t>
     </r>
@@ -111,7 +111,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -138,7 +138,7 @@
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="128"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -146,19 +146,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="128"/>
     </font>
     <font>
       <sz val="12"/>
@@ -171,7 +158,7 @@
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="128"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -229,15 +216,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -245,7 +232,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -270,17 +257,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P49"/>
+  <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -336,18 +323,20 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
-        <v>44070</v>
+        <v>44076</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="F2" s="5"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6" t="n">
@@ -356,7 +345,9 @@
       <c r="I2" s="6"/>
       <c r="J2" s="7"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
+      <c r="L2" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="M2" s="7" t="n">
         <v>1</v>
       </c>
@@ -369,26 +360,26 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
-        <v>44069</v>
+        <v>44075</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="6"/>
+      <c r="K3" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="7" t="n">
@@ -402,10 +393,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
-        <v>44068</v>
+        <v>44074</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>3</v>
@@ -413,20 +404,20 @@
       <c r="D4" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="5" t="n">
-        <v>1</v>
-      </c>
+      <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
       <c r="K4" s="6"/>
       <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
+      <c r="M4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="O4" s="6" t="n">
         <f aca="false">IF(SUM(D4:N4)=C4,1,0)</f>
         <v>1</v>
@@ -435,29 +426,31 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
-        <v>44067</v>
+        <v>44073</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="6"/>
+      <c r="K5" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
+      <c r="N5" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="O5" s="6" t="n">
         <f aca="false">IF(SUM(D5:N5)=C5,1,0)</f>
         <v>1</v>
@@ -466,18 +459,20 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
-        <v>44066</v>
+        <v>44072</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="F6" s="5"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="n">
@@ -485,94 +480,104 @@
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="K6" s="6"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
-      <c r="N6" s="7" t="n">
-        <v>1</v>
-      </c>
+      <c r="N6" s="7"/>
       <c r="O6" s="6" t="n">
         <f aca="false">IF(SUM(D6:N6)=C6,1,0)</f>
         <v>1</v>
       </c>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
-        <v>44065</v>
+        <v>44071</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="K7" s="6"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
+      <c r="N7" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="O7" s="6" t="n">
         <f aca="false">IF(SUM(D7:N7)=C7,1,0)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
-        <v>44064</v>
+        <v>44070</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="6" t="n">
         <v>1</v>
       </c>
+      <c r="I8" s="6"/>
       <c r="J8" s="7"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="M8" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="N8" s="7"/>
       <c r="O8" s="6" t="n">
         <f aca="false">IF(SUM(D8:N8)=C8,1,0)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
-        <v>44063</v>
+        <v>44069</v>
       </c>
       <c r="B9" s="5" t="n">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="G9" s="6"/>
       <c r="H9" s="6" t="n">
         <v>1</v>
       </c>
+      <c r="I9" s="6"/>
       <c r="J9" s="7"/>
+      <c r="K9" s="6"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7" t="n">
@@ -582,78 +587,78 @@
         <f aca="false">IF(SUM(D9:N9)=C9,1,0)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
-        <v>44062</v>
+        <v>44068</v>
       </c>
       <c r="B10" s="5" t="n">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="6" t="n">
         <v>1</v>
       </c>
+      <c r="I10" s="6"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="K10" s="6"/>
       <c r="L10" s="7"/>
-      <c r="M10" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N10" s="7" t="n">
-        <v>1</v>
-      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
       <c r="O10" s="6" t="n">
         <f aca="false">IF(SUM(D10:N10)=C10,1,0)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
-        <v>44061</v>
+        <v>44067</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D11" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="J11" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L11" s="7" t="n">
-        <v>1</v>
-      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="7"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
       <c r="O11" s="6" t="n">
         <f aca="false">IF(SUM(D11:N11)=C11,1,0)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
-        <v>44060</v>
+        <v>44066</v>
       </c>
       <c r="B12" s="5" t="n">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="C12" s="5" t="n">
         <v>4</v>
@@ -663,48 +668,48 @@
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="6" t="n">
         <v>1</v>
       </c>
+      <c r="I12" s="6"/>
       <c r="J12" s="7"/>
       <c r="K12" s="6" t="n">
         <v>1</v>
       </c>
       <c r="L12" s="7"/>
-      <c r="M12" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="O12" s="6" t="n">
         <f aca="false">IF(SUM(D12:N12)=C12,1,0)</f>
         <v>1</v>
       </c>
+      <c r="P12" s="2"/>
     </row>
     <row r="13" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
-        <v>44059</v>
+        <v>44065</v>
       </c>
       <c r="B13" s="5" t="n">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="C13" s="5" t="n">
-        <f aca="false">B13-B14</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D13" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="H13" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="L13" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="F13" s="5"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
       <c r="O13" s="6" t="n">
         <f aca="false">IF(SUM(D13:N13)=C13,1,0)</f>
         <v>1</v>
@@ -712,23 +717,24 @@
     </row>
     <row r="14" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
-        <v>44058</v>
+        <v>44064</v>
       </c>
       <c r="B14" s="5" t="n">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="C14" s="5" t="n">
-        <f aca="false">B14-B15</f>
-        <v>2</v>
-      </c>
-      <c r="D14" s="5" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="I14" s="7"/>
-      <c r="K14" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="F14" s="5"/>
+      <c r="H14" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
       <c r="O14" s="6" t="n">
         <f aca="false">IF(SUM(D14:N14)=C14,1,0)</f>
         <v>1</v>
@@ -736,23 +742,29 @@
     </row>
     <row r="15" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
-        <v>44057</v>
+        <v>44063</v>
       </c>
       <c r="B15" s="5" t="n">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C15" s="5" t="n">
-        <f aca="false">B15-B16</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="F15" s="5"/>
       <c r="G15" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7" t="n">
         <v>1</v>
       </c>
       <c r="O15" s="6" t="n">
@@ -762,21 +774,32 @@
     </row>
     <row r="16" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
-        <v>44056</v>
+        <v>44062</v>
       </c>
       <c r="B16" s="5" t="n">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="C16" s="5" t="n">
-        <f aca="false">B16-B17</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="6" t="n">
-        <v>2</v>
+      <c r="F16" s="5"/>
+      <c r="H16" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="7"/>
+      <c r="K16" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="O16" s="6" t="n">
         <f aca="false">IF(SUM(D16:N16)=C16,1,0)</f>
@@ -785,22 +808,30 @@
     </row>
     <row r="17" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
-        <v>44054</v>
+        <v>44061</v>
       </c>
       <c r="B17" s="5" t="n">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C17" s="5" t="n">
-        <f aca="false">B17-B18</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="F17" s="5"/>
+      <c r="H17" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
       <c r="O17" s="6" t="n">
         <f aca="false">IF(SUM(D17:N17)=C17,1,0)</f>
         <v>1</v>
@@ -808,19 +839,31 @@
     </row>
     <row r="18" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="n">
-        <v>44052</v>
+        <v>44060</v>
       </c>
       <c r="B18" s="5" t="n">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="C18" s="5" t="n">
-        <f aca="false">B18-B19</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="H18" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" s="7"/>
+      <c r="K18" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N18" s="7"/>
       <c r="O18" s="6" t="n">
         <f aca="false">IF(SUM(D18:N18)=C18,1,0)</f>
         <v>1</v>
@@ -828,14 +871,14 @@
     </row>
     <row r="19" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
-        <v>44051</v>
+        <v>44059</v>
       </c>
       <c r="B19" s="5" t="n">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="C19" s="5" t="n">
         <f aca="false">B19-B20</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D19" s="5" t="n">
         <v>1</v>
@@ -844,6 +887,13 @@
       <c r="H19" s="6" t="n">
         <v>1</v>
       </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="O19" s="6" t="n">
         <f aca="false">IF(SUM(D19:N19)=C19,1,0)</f>
         <v>1</v>
@@ -851,23 +901,21 @@
     </row>
     <row r="20" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
-        <v>44048</v>
+        <v>44058</v>
       </c>
       <c r="B20" s="5" t="n">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C20" s="5" t="n">
         <f aca="false">B20-B21</f>
         <v>2</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="5"/>
-      <c r="G20" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="6" t="n">
+      <c r="I20" s="7"/>
+      <c r="K20" s="6" t="n">
         <v>1</v>
       </c>
       <c r="O20" s="6" t="n">
@@ -877,23 +925,23 @@
     </row>
     <row r="21" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
-        <v>44046</v>
+        <v>44057</v>
       </c>
       <c r="B21" s="5" t="n">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C21" s="5" t="n">
         <f aca="false">B21-B22</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D21" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H21" s="6" t="n">
+      <c r="G21" s="6" t="n">
         <v>1</v>
       </c>
       <c r="O21" s="6" t="n">
@@ -903,18 +951,22 @@
     </row>
     <row r="22" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="n">
-        <v>44045</v>
+        <v>44056</v>
       </c>
       <c r="B22" s="5" t="n">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C22" s="5" t="n">
-        <v>1</v>
+        <f aca="false">B22-B23</f>
+        <v>2</v>
       </c>
       <c r="D22" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="5"/>
+      <c r="F22" s="6" t="n">
+        <v>2</v>
+      </c>
       <c r="O22" s="6" t="n">
         <f aca="false">IF(SUM(D22:N22)=C22,1,0)</f>
         <v>1</v>
@@ -922,18 +974,22 @@
     </row>
     <row r="23" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="n">
-        <v>44043</v>
+        <v>44054</v>
       </c>
       <c r="B23" s="5" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C23" s="5" t="n">
-        <v>2</v>
+        <f aca="false">B23-B24</f>
+        <v>1</v>
       </c>
       <c r="D23" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E23" s="5"/>
+      <c r="F23" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="O23" s="6" t="n">
         <f aca="false">IF(SUM(D23:N23)=C23,1,0)</f>
         <v>1</v>
@@ -941,17 +997,17 @@
     </row>
     <row r="24" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="n">
-        <v>44042</v>
+        <v>44052</v>
       </c>
       <c r="B24" s="5" t="n">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C24" s="5" t="n">
         <f aca="false">B24-B25</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" s="5"/>
       <c r="O24" s="6" t="n">
@@ -959,12 +1015,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" s="6" customFormat="true" ht="35.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="n">
-        <v>44039</v>
+        <v>44051</v>
       </c>
       <c r="B25" s="5" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C25" s="5" t="n">
         <f aca="false">B25-B26</f>
@@ -974,33 +1030,33 @@
         <v>1</v>
       </c>
       <c r="E25" s="5"/>
-      <c r="K25" s="6" t="n">
+      <c r="H25" s="6" t="n">
         <v>1</v>
       </c>
       <c r="O25" s="6" t="n">
         <f aca="false">IF(SUM(D25:N25)=C25,1,0)</f>
         <v>1</v>
       </c>
-      <c r="P25" s="8" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="26" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="n">
-        <v>44038</v>
+        <v>44048</v>
       </c>
       <c r="B26" s="5" t="n">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C26" s="5" t="n">
         <f aca="false">B26-B27</f>
         <v>2</v>
       </c>
       <c r="D26" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="5"/>
-      <c r="F26" s="6" t="n">
+      <c r="G26" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" s="6" t="n">
         <v>1</v>
       </c>
       <c r="O26" s="6" t="n">
@@ -1010,19 +1066,25 @@
     </row>
     <row r="27" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="n">
-        <v>44037</v>
+        <v>44046</v>
       </c>
       <c r="B27" s="5" t="n">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C27" s="5" t="n">
         <f aca="false">B27-B28</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="5"/>
+      <c r="F27" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="O27" s="6" t="n">
         <f aca="false">IF(SUM(D27:N27)=C27,1,0)</f>
         <v>1</v>
@@ -1030,17 +1092,16 @@
     </row>
     <row r="28" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="n">
-        <v>44035</v>
+        <v>44045</v>
       </c>
       <c r="B28" s="5" t="n">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C28" s="5" t="n">
-        <f aca="false">B28-B29</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D28" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E28" s="5"/>
       <c r="O28" s="6" t="n">
@@ -1050,17 +1111,16 @@
     </row>
     <row r="29" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="n">
-        <v>44034</v>
+        <v>44043</v>
       </c>
       <c r="B29" s="5" t="n">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C29" s="5" t="n">
-        <f aca="false">B29-B30</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" s="5"/>
       <c r="O29" s="6" t="n">
@@ -1070,17 +1130,17 @@
     </row>
     <row r="30" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="n">
-        <v>44033</v>
+        <v>44042</v>
       </c>
       <c r="B30" s="5" t="n">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C30" s="5" t="n">
         <f aca="false">B30-B31</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" s="5"/>
       <c r="O30" s="6" t="n">
@@ -1088,41 +1148,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" s="6" customFormat="true" ht="35.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="n">
-        <v>44032</v>
+        <v>44039</v>
       </c>
       <c r="B31" s="5" t="n">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C31" s="5" t="n">
         <f aca="false">B31-B32</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D31" s="5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E31" s="5"/>
+      <c r="K31" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="O31" s="6" t="n">
         <f aca="false">IF(SUM(D31:N31)=C31,1,0)</f>
         <v>1</v>
       </c>
+      <c r="P31" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="32" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="n">
-        <v>44029</v>
+        <v>44038</v>
       </c>
       <c r="B32" s="5" t="n">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C32" s="5" t="n">
         <f aca="false">B32-B33</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D32" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E32" s="5"/>
+      <c r="F32" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="O32" s="6" t="n">
         <f aca="false">IF(SUM(D32:N32)=C32,1,0)</f>
         <v>1</v>
@@ -1130,21 +1199,19 @@
     </row>
     <row r="33" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="n">
-        <v>44027</v>
+        <v>44037</v>
       </c>
       <c r="B33" s="5" t="n">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C33" s="5" t="n">
         <f aca="false">B33-B34</f>
         <v>1</v>
       </c>
       <c r="D33" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" s="5" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E33" s="5"/>
       <c r="O33" s="6" t="n">
         <f aca="false">IF(SUM(D33:N33)=C33,1,0)</f>
         <v>1</v>
@@ -1152,17 +1219,17 @@
     </row>
     <row r="34" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="n">
-        <v>44026</v>
+        <v>44035</v>
       </c>
       <c r="B34" s="5" t="n">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C34" s="5" t="n">
         <f aca="false">B34-B35</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D34" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E34" s="5"/>
       <c r="O34" s="6" t="n">
@@ -1172,17 +1239,17 @@
     </row>
     <row r="35" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="n">
-        <v>44025</v>
+        <v>44034</v>
       </c>
       <c r="B35" s="5" t="n">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C35" s="5" t="n">
         <f aca="false">B35-B36</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D35" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E35" s="5"/>
       <c r="O35" s="6" t="n">
@@ -1192,10 +1259,10 @@
     </row>
     <row r="36" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="n">
-        <v>44022</v>
+        <v>44033</v>
       </c>
       <c r="B36" s="5" t="n">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C36" s="5" t="n">
         <f aca="false">B36-B37</f>
@@ -1212,17 +1279,17 @@
     </row>
     <row r="37" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="n">
-        <v>44018</v>
+        <v>44032</v>
       </c>
       <c r="B37" s="5" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C37" s="5" t="n">
         <f aca="false">B37-B38</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D37" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E37" s="5"/>
       <c r="O37" s="6" t="n">
@@ -1232,21 +1299,19 @@
     </row>
     <row r="38" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="n">
-        <v>44017</v>
+        <v>44029</v>
       </c>
       <c r="B38" s="5" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C38" s="5" t="n">
         <f aca="false">B38-B39</f>
         <v>3</v>
       </c>
       <c r="D38" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E38" s="5" t="n">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E38" s="5"/>
       <c r="O38" s="6" t="n">
         <f aca="false">IF(SUM(D38:N38)=C38,1,0)</f>
         <v>1</v>
@@ -1254,19 +1319,21 @@
     </row>
     <row r="39" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="n">
-        <v>44015</v>
+        <v>44027</v>
       </c>
       <c r="B39" s="5" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C39" s="5" t="n">
         <f aca="false">B39-B40</f>
         <v>1</v>
       </c>
       <c r="D39" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E39" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="O39" s="6" t="n">
         <f aca="false">IF(SUM(D39:N39)=C39,1,0)</f>
         <v>1</v>
@@ -1274,43 +1341,37 @@
     </row>
     <row r="40" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="n">
-        <v>44009</v>
+        <v>44026</v>
       </c>
       <c r="B40" s="5" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C40" s="5" t="n">
         <f aca="false">B40-B41</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D40" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E40" s="5"/>
-      <c r="K40" s="6" t="n">
-        <v>1</v>
-      </c>
       <c r="O40" s="6" t="n">
         <f aca="false">IF(SUM(D40:N40)=C40,1,0)</f>
         <v>1</v>
       </c>
-      <c r="P40" s="5" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="41" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="n">
-        <v>44008</v>
+        <v>44025</v>
       </c>
       <c r="B41" s="5" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C41" s="5" t="n">
         <f aca="false">B41-B42</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D41" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E41" s="5"/>
       <c r="O41" s="6" t="n">
@@ -1320,22 +1381,19 @@
     </row>
     <row r="42" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="n">
-        <v>43999</v>
+        <v>44022</v>
       </c>
       <c r="B42" s="5" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C42" s="5" t="n">
         <f aca="false">B42-B43</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D42" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E42" s="5"/>
-      <c r="I42" s="6" t="n">
-        <v>1</v>
-      </c>
       <c r="O42" s="6" t="n">
         <f aca="false">IF(SUM(D42:N42)=C42,1,0)</f>
         <v>1</v>
@@ -1343,10 +1401,10 @@
     </row>
     <row r="43" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="n">
-        <v>43984</v>
+        <v>44018</v>
       </c>
       <c r="B43" s="5" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C43" s="5" t="n">
         <f aca="false">B43-B44</f>
@@ -1363,19 +1421,21 @@
     </row>
     <row r="44" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="n">
-        <v>43982</v>
+        <v>44017</v>
       </c>
       <c r="B44" s="5" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C44" s="5" t="n">
         <f aca="false">B44-B45</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D44" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E44" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="E44" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="O44" s="6" t="n">
         <f aca="false">IF(SUM(D44:N44)=C44,1,0)</f>
         <v>1</v>
@@ -1383,10 +1443,10 @@
     </row>
     <row r="45" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="n">
-        <v>43973</v>
+        <v>44015</v>
       </c>
       <c r="B45" s="5" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C45" s="5" t="n">
         <f aca="false">B45-B46</f>
@@ -1403,39 +1463,45 @@
     </row>
     <row r="46" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="n">
-        <v>43940</v>
+        <v>44009</v>
       </c>
       <c r="B46" s="5" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C46" s="5" t="n">
+        <f aca="false">B46-B47</f>
         <v>1</v>
       </c>
       <c r="D46" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46" s="5"/>
+      <c r="K46" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="O46" s="6" t="n">
         <f aca="false">IF(SUM(D46:N46)=C46,1,0)</f>
         <v>1</v>
       </c>
+      <c r="P46" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="47" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="n">
-        <v>43920</v>
+        <v>44008</v>
       </c>
       <c r="B47" s="5" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C47" s="5" t="n">
+        <f aca="false">B47-B48</f>
         <v>1</v>
       </c>
       <c r="D47" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" s="5" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E47" s="5"/>
       <c r="O47" s="6" t="n">
         <f aca="false">IF(SUM(D47:N47)=C47,1,0)</f>
         <v>1</v>
@@ -1443,15 +1509,20 @@
     </row>
     <row r="48" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="n">
-        <v>43919</v>
-      </c>
-      <c r="B48" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C48" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D48" s="6" t="n">
+        <v>43999</v>
+      </c>
+      <c r="B48" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="C48" s="5" t="n">
+        <f aca="false">B48-B49</f>
+        <v>1</v>
+      </c>
+      <c r="D48" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" s="5"/>
+      <c r="I48" s="6" t="n">
         <v>1</v>
       </c>
       <c r="O48" s="6" t="n">
@@ -1459,56 +1530,174 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2" t="n">
-        <f aca="false">SUM(C$5:C48)</f>
-        <v>92</v>
-      </c>
-      <c r="D49" s="2" t="n">
-        <f aca="false">SUM(D$5:D48)</f>
-        <v>52</v>
-      </c>
-      <c r="E49" s="2" t="n">
-        <f aca="false">SUM(E$5:E48)</f>
-        <v>3</v>
-      </c>
-      <c r="F49" s="2" t="n">
-        <f aca="false">SUM(F$5:F48)</f>
+    <row r="49" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4" t="n">
+        <v>43984</v>
+      </c>
+      <c r="B49" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G49" s="2" t="n">
-        <f aca="false">SUM(G$5:G48)</f>
-        <v>3</v>
-      </c>
-      <c r="H49" s="2" t="n">
-        <f aca="false">SUM(H$5:H48)</f>
-        <v>11</v>
-      </c>
-      <c r="I49" s="2" t="n">
-        <f aca="false">SUM(I$5:I48)</f>
-        <v>1</v>
-      </c>
-      <c r="J49" s="2" t="n">
-        <f aca="false">SUM(J$5:J48)</f>
-        <v>2</v>
-      </c>
-      <c r="K49" s="2" t="n">
-        <f aca="false">SUM(K$5:K48)</f>
-        <v>7</v>
-      </c>
-      <c r="L49" s="2" t="n">
-        <f aca="false">SUM(L$5:L48)</f>
-        <v>2</v>
-      </c>
-      <c r="M49" s="2" t="n">
-        <f aca="false">SUM(M$5:M48)</f>
-        <v>2</v>
-      </c>
-      <c r="N49" s="2" t="n">
-        <f aca="false">SUM(N$5:N48)</f>
-        <v>3</v>
+      <c r="C49" s="5" t="n">
+        <f aca="false">B49-B50</f>
+        <v>1</v>
+      </c>
+      <c r="D49" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E49" s="5"/>
+      <c r="O49" s="6" t="n">
+        <f aca="false">IF(SUM(D49:N49)=C49,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4" t="n">
+        <v>43982</v>
+      </c>
+      <c r="B50" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C50" s="5" t="n">
+        <f aca="false">B50-B51</f>
+        <v>1</v>
+      </c>
+      <c r="D50" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" s="5"/>
+      <c r="O50" s="6" t="n">
+        <f aca="false">IF(SUM(D50:N50)=C50,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="4" t="n">
+        <v>43973</v>
+      </c>
+      <c r="B51" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C51" s="5" t="n">
+        <f aca="false">B51-B52</f>
+        <v>1</v>
+      </c>
+      <c r="D51" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="O51" s="6" t="n">
+        <f aca="false">IF(SUM(D51:N51)=C51,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="n">
+        <v>43940</v>
+      </c>
+      <c r="B52" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C52" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" s="5"/>
+      <c r="O52" s="6" t="n">
+        <f aca="false">IF(SUM(D52:N52)=C52,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4" t="n">
+        <v>43920</v>
+      </c>
+      <c r="B53" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C53" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O53" s="6" t="n">
+        <f aca="false">IF(SUM(D53:N53)=C53,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="4" t="n">
+        <v>43919</v>
+      </c>
+      <c r="B54" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C54" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D54" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O54" s="6" t="n">
+        <f aca="false">IF(SUM(D54:N54)=C54,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2" t="n">
+        <f aca="false">SUM(C$2:C54)</f>
+        <v>120</v>
+      </c>
+      <c r="D55" s="2" t="n">
+        <f aca="false">SUM(D$2:D54)</f>
+        <v>60</v>
+      </c>
+      <c r="E55" s="2" t="n">
+        <f aca="false">SUM(E$2:E54)</f>
+        <v>6</v>
+      </c>
+      <c r="F55" s="2" t="n">
+        <f aca="false">SUM(F$2:F54)</f>
+        <v>6</v>
+      </c>
+      <c r="G55" s="2" t="n">
+        <f aca="false">SUM(G$2:G54)</f>
+        <v>3</v>
+      </c>
+      <c r="H55" s="2" t="n">
+        <f aca="false">SUM(H$2:H54)</f>
+        <v>17</v>
+      </c>
+      <c r="I55" s="2" t="n">
+        <f aca="false">SUM(I$2:I54)</f>
+        <v>1</v>
+      </c>
+      <c r="J55" s="2" t="n">
+        <f aca="false">SUM(J$2:J54)</f>
+        <v>2</v>
+      </c>
+      <c r="K55" s="2" t="n">
+        <f aca="false">SUM(K$2:K54)</f>
+        <v>9</v>
+      </c>
+      <c r="L55" s="2" t="n">
+        <f aca="false">SUM(L$2:L54)</f>
+        <v>3</v>
+      </c>
+      <c r="M55" s="2" t="n">
+        <f aca="false">SUM(M$2:M54)</f>
+        <v>5</v>
+      </c>
+      <c r="N55" s="2" t="n">
+        <f aca="false">SUM(N$2:N54)</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
and update the run script
</commit_message>
<xml_diff>
--- a/src/syria_under_reporting/death_sheet.xlsx
+++ b/src/syria_under_reporting/death_sheet.xlsx
@@ -267,7 +267,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -328,7 +328,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
-        <v>44052</v>
+        <v>44083</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>143</v>

</xml_diff>